<commit_message>
fix some issue related to parallel ref
</commit_message>
<xml_diff>
--- a/src/main/resources/excels/android/Check CRUD supplier.xlsx
+++ b/src/main/resources/excels/android/Check CRUD supplier.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="25">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -472,6 +475,9 @@
       <c r="D2" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="E2" t="s" s="0">
+        <v>23</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="91.2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
@@ -486,6 +492,9 @@
       <c r="D3" s="5" t="s">
         <v>11</v>
       </c>
+      <c r="E3" t="s" s="0">
+        <v>23</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="34.200000000000003" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
@@ -500,6 +509,9 @@
       <c r="D4" s="5" t="s">
         <v>21</v>
       </c>
+      <c r="E4" t="s" s="0">
+        <v>23</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="34.200000000000003" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -513,6 +525,9 @@
       </c>
       <c r="D5" s="5" t="s">
         <v>21</v>
+      </c>
+      <c r="E5" t="s" s="0">
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="34.200000000000003" x14ac:dyDescent="0.25">

</xml_diff>